<commit_message>
volt profile section data dump complete
</commit_message>
<xml_diff>
--- a/remc_report_config.xlsx
+++ b/remc_report_config.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="section_1" sheetId="1" r:id="rId1"/>
-    <sheet name="section_2" sheetId="2" r:id="rId2"/>
-    <sheet name="section_3" sheetId="3" r:id="rId3"/>
+    <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
+    <sheet name="ists_gen" sheetId="2" r:id="rId2"/>
+    <sheet name="state_gen" sheetId="3" r:id="rId3"/>
+    <sheet name="volt_profile" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -191,6 +192,33 @@
   </si>
   <si>
     <t>WREMCPRI.SCADA01.00045129,WREMCPRI.SCADA01.00046848</t>
+  </si>
+  <si>
+    <t>400_kv_pnt</t>
+  </si>
+  <si>
+    <t>220_kv_pnt</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00016226</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00016228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BACHHAU </t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00016241</t>
+  </si>
+  <si>
+    <t>WREMCPRI.SCADA01.00016243</t>
+  </si>
+  <si>
+    <t>REWA</t>
+  </si>
+  <si>
+    <t>Dummay Row</t>
   </si>
 </sst>
 </file>
@@ -232,9 +260,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,7 +678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -808,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,4 +951,74 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
graph data fetch start
</commit_message>
<xml_diff>
--- a/remc_report_config.xlsx
+++ b/remc_report_config.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="regional_profile" sheetId="1" r:id="rId1"/>
     <sheet name="ists_gen" sheetId="2" r:id="rId2"/>
     <sheet name="state_gen" sheetId="3" r:id="rId3"/>
     <sheet name="volt_profile" sheetId="4" r:id="rId4"/>
+    <sheet name="graph_data" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -219,6 +220,21 @@
   </si>
   <si>
     <t>Dummay Row</t>
+  </si>
+  <si>
+    <t>day_offset</t>
+  </si>
+  <si>
+    <t>pnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WR ISTS Total Schedule </t>
+  </si>
+  <si>
+    <t>WR ISTS  Total Actual</t>
+  </si>
+  <si>
+    <t>WR ISTS  Total Actual Prev</t>
   </si>
 </sst>
 </file>
@@ -678,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,4 +1037,77 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>